<commit_message>
implement rolling horizon simulation
</commit_message>
<xml_diff>
--- a/Instances/04_NonStationary_b2_fe25_en_rk50_ll0_l20_HFalse_c2.xlsx
+++ b/Instances/04_NonStationary_b2_fe25_en_rk50_ll0_l20_HFalse_c2.xlsx
@@ -2279,7 +2279,7 @@
         <v>0.085536</v>
       </c>
       <c r="E2" t="n">
-        <v>11.6408512</v>
+        <v>11.7029088</v>
       </c>
       <c r="F2" t="n">
         <v>0.171072</v>
@@ -2311,7 +2311,7 @@
         <v>0.083916</v>
       </c>
       <c r="E3" t="n">
-        <v>2.171936</v>
+        <v>2.1871904</v>
       </c>
       <c r="F3" t="n">
         <v>0.167832</v>
@@ -2343,7 +2343,7 @@
         <v>0.08401600000000001</v>
       </c>
       <c r="E4" t="n">
-        <v>0.9253279999999999</v>
+        <v>0.891504</v>
       </c>
       <c r="F4" t="n">
         <v>0.168032</v>
@@ -2375,7 +2375,7 @@
         <v>0.08357200000000001</v>
       </c>
       <c r="E5" t="n">
-        <v>1.432296</v>
+        <v>1.414512</v>
       </c>
       <c r="F5" t="n">
         <v>0.167144</v>
@@ -2407,7 +2407,7 @@
         <v>0.081992</v>
       </c>
       <c r="E6" t="n">
-        <v>0.9675328000000001</v>
+        <v>0.9700991999999999</v>
       </c>
       <c r="F6" t="n">
         <v>0.163984</v>
@@ -2439,7 +2439,7 @@
         <v>0.082176</v>
       </c>
       <c r="E7" t="n">
-        <v>0.2823648</v>
+        <v>0.2920128</v>
       </c>
       <c r="F7" t="n">
         <v>0.164352</v>
@@ -2471,7 +2471,7 @@
         <v>0.08182400000000001</v>
       </c>
       <c r="E8" t="n">
-        <v>0.09250560000000001</v>
+        <v>0.0988416</v>
       </c>
       <c r="F8" t="n">
         <v>0.163648</v>
@@ -2497,13 +2497,13 @@
         <v>1</v>
       </c>
       <c r="C9" t="n">
-        <v>840</v>
+        <v>839</v>
       </c>
       <c r="D9" t="n">
         <v>0.086564</v>
       </c>
       <c r="E9" t="n">
-        <v>0.8610528000000001</v>
+        <v>0.8602304</v>
       </c>
       <c r="F9" t="n">
         <v>0.173128</v>
@@ -2529,13 +2529,13 @@
         <v>1</v>
       </c>
       <c r="C10" t="n">
-        <v>598</v>
+        <v>607</v>
       </c>
       <c r="D10" t="n">
         <v>0.0864</v>
       </c>
       <c r="E10" t="n">
-        <v>0.5173632</v>
+        <v>0.5215104</v>
       </c>
       <c r="F10" t="n">
         <v>0.1728</v>
@@ -2561,13 +2561,13 @@
         <v>1</v>
       </c>
       <c r="C11" t="n">
-        <v>1789</v>
+        <v>1803</v>
       </c>
       <c r="D11" t="n">
         <v>0.085956</v>
       </c>
       <c r="E11" t="n">
-        <v>0.7518</v>
+        <v>0.757344</v>
       </c>
       <c r="F11" t="n">
         <v>0.171912</v>
@@ -2593,13 +2593,13 @@
         <v>1</v>
       </c>
       <c r="C12" t="n">
-        <v>413</v>
+        <v>418</v>
       </c>
       <c r="D12" t="n">
         <v>0.08652000000000001</v>
       </c>
       <c r="E12" t="n">
-        <v>1.2346224</v>
+        <v>1.2192928</v>
       </c>
       <c r="F12" t="n">
         <v>0.17304</v>
@@ -2625,13 +2625,13 @@
         <v>1</v>
       </c>
       <c r="C13" t="n">
-        <v>3227</v>
+        <v>3237</v>
       </c>
       <c r="D13" t="n">
         <v>0.081928</v>
       </c>
       <c r="E13" t="n">
-        <v>12.51843199999999</v>
+        <v>12.58516799999999</v>
       </c>
       <c r="F13" t="n">
         <v>0.163856</v>
@@ -2657,13 +2657,13 @@
         <v>1</v>
       </c>
       <c r="C14" t="n">
-        <v>1197</v>
+        <v>1211</v>
       </c>
       <c r="D14" t="n">
         <v>0.08210000000000001</v>
       </c>
       <c r="E14" t="n">
-        <v>4.846192000000001</v>
+        <v>4.880228800000001</v>
       </c>
       <c r="F14" t="n">
         <v>0.1642</v>
@@ -2689,13 +2689,13 @@
         <v>1</v>
       </c>
       <c r="C15" t="n">
-        <v>305</v>
+        <v>300</v>
       </c>
       <c r="D15" t="n">
         <v>0.08099600000000001</v>
       </c>
       <c r="E15" t="n">
-        <v>0.9032671999999999</v>
+        <v>0.8702496</v>
       </c>
       <c r="F15" t="n">
         <v>0.161992</v>
@@ -2721,13 +2721,13 @@
         <v>1</v>
       </c>
       <c r="C16" t="n">
-        <v>429</v>
+        <v>413</v>
       </c>
       <c r="D16" t="n">
         <v>0.080152</v>
       </c>
       <c r="E16" t="n">
-        <v>0.8811552</v>
+        <v>0.8702144000000001</v>
       </c>
       <c r="F16" t="n">
         <v>0.160304</v>
@@ -2753,13 +2753,13 @@
         <v>1</v>
       </c>
       <c r="C17" t="n">
-        <v>607</v>
+        <v>609</v>
       </c>
       <c r="D17" t="n">
         <v>0.080388</v>
       </c>
       <c r="E17" t="n">
-        <v>1.411488</v>
+        <v>1.415232</v>
       </c>
       <c r="F17" t="n">
         <v>0.160776</v>
@@ -2785,13 +2785,13 @@
         <v>1</v>
       </c>
       <c r="C18" t="n">
-        <v>176</v>
+        <v>181</v>
       </c>
       <c r="D18" t="n">
         <v>0.080568</v>
       </c>
       <c r="E18" t="n">
-        <v>0.442512</v>
+        <v>0.457632</v>
       </c>
       <c r="F18" t="n">
         <v>0.161136</v>
@@ -2817,13 +2817,13 @@
         <v>1</v>
       </c>
       <c r="C19" t="n">
-        <v>52</v>
+        <v>60</v>
       </c>
       <c r="D19" t="n">
         <v>0.08024000000000001</v>
       </c>
       <c r="E19" t="n">
-        <v>0.1280128</v>
+        <v>0.1367808</v>
       </c>
       <c r="F19" t="n">
         <v>0.16048</v>
@@ -2855,7 +2855,7 @@
         <v>0.01052</v>
       </c>
       <c r="E20" t="n">
-        <v>62.960096</v>
+        <v>63.17891200000001</v>
       </c>
       <c r="F20" t="n">
         <v>0.02104</v>
@@ -2887,7 +2887,7 @@
         <v>0.011168</v>
       </c>
       <c r="E21" t="n">
-        <v>66.8382464</v>
+        <v>67.0705408</v>
       </c>
       <c r="F21" t="n">
         <v>0.022336</v>
@@ -2919,7 +2919,7 @@
         <v>0.013824</v>
       </c>
       <c r="E22" t="n">
-        <v>82.7338752</v>
+        <v>83.02141440000001</v>
       </c>
       <c r="F22" t="n">
         <v>0.027648</v>
@@ -2951,7 +2951,7 @@
         <v>0.042536</v>
       </c>
       <c r="E23" t="n">
-        <v>254.5694528</v>
+        <v>255.4542016</v>
       </c>
       <c r="F23" t="n">
         <v>0.08507200000000001</v>
@@ -3064,34 +3064,34 @@
         <v>0</v>
       </c>
       <c r="C2" t="n">
-        <v>601</v>
+        <v>594</v>
       </c>
       <c r="D2" t="n">
-        <v>151</v>
+        <v>137</v>
       </c>
       <c r="E2" t="n">
         <v>0</v>
       </c>
       <c r="F2" t="n">
-        <v>295</v>
+        <v>300</v>
       </c>
       <c r="G2" t="n">
-        <v>86</v>
+        <v>93</v>
       </c>
       <c r="H2" t="n">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="I2" t="n">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="J2" t="n">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="K2" t="n">
-        <v>898</v>
+        <v>895</v>
       </c>
       <c r="L2" t="n">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="M2" t="n">
         <v>0</v>
@@ -3135,34 +3135,34 @@
         <v>0</v>
       </c>
       <c r="C3" t="n">
-        <v>598</v>
+        <v>603</v>
       </c>
       <c r="D3" t="n">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="E3" t="n">
         <v>0</v>
       </c>
       <c r="F3" t="n">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="G3" t="n">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="H3" t="n">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="I3" t="n">
         <v>421</v>
       </c>
       <c r="J3" t="n">
-        <v>297</v>
+        <v>305</v>
       </c>
       <c r="K3" t="n">
-        <v>891</v>
+        <v>908</v>
       </c>
       <c r="L3" t="n">
-        <v>203</v>
+        <v>212</v>
       </c>
       <c r="M3" t="n">
         <v>0</v>
@@ -3206,22 +3206,22 @@
         <v>0</v>
       </c>
       <c r="C4" t="n">
-        <v>600</v>
+        <v>610</v>
       </c>
       <c r="D4" t="n">
-        <v>154</v>
+        <v>145</v>
       </c>
       <c r="E4" t="n">
         <v>0</v>
       </c>
       <c r="F4" t="n">
-        <v>302</v>
+        <v>305</v>
       </c>
       <c r="G4" t="n">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="H4" t="n">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="I4" t="n">
         <v>418</v>
@@ -3230,10 +3230,10 @@
         <v>298</v>
       </c>
       <c r="K4" t="n">
-        <v>899</v>
+        <v>903</v>
       </c>
       <c r="L4" t="n">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="M4" t="n">
         <v>0</v>
@@ -3277,34 +3277,34 @@
         <v>0</v>
       </c>
       <c r="C5" t="n">
-        <v>597</v>
+        <v>601</v>
       </c>
       <c r="D5" t="n">
-        <v>151</v>
+        <v>155</v>
       </c>
       <c r="E5" t="n">
         <v>0</v>
       </c>
       <c r="F5" t="n">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="G5" t="n">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="H5" t="n">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="I5" t="n">
-        <v>418</v>
+        <v>415</v>
       </c>
       <c r="J5" t="n">
-        <v>304</v>
+        <v>300</v>
       </c>
       <c r="K5" t="n">
-        <v>890</v>
+        <v>903</v>
       </c>
       <c r="L5" t="n">
-        <v>213</v>
+        <v>202</v>
       </c>
       <c r="M5" t="n">
         <v>0</v>
@@ -3348,34 +3348,34 @@
         <v>0</v>
       </c>
       <c r="C6" t="n">
-        <v>594</v>
+        <v>603</v>
       </c>
       <c r="D6" t="n">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="E6" t="n">
         <v>0</v>
       </c>
       <c r="F6" t="n">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="G6" t="n">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="H6" t="n">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="I6" t="n">
-        <v>418</v>
+        <v>420</v>
       </c>
       <c r="J6" t="n">
-        <v>297</v>
+        <v>304</v>
       </c>
       <c r="K6" t="n">
-        <v>897</v>
+        <v>899</v>
       </c>
       <c r="L6" t="n">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="M6" t="n">
         <v>0</v>
@@ -3506,34 +3506,34 @@
         <v>0</v>
       </c>
       <c r="C2" t="n">
-        <v>75.125</v>
+        <v>74.25</v>
       </c>
       <c r="D2" t="n">
-        <v>18.875</v>
+        <v>17.125</v>
       </c>
       <c r="E2" t="n">
         <v>0</v>
       </c>
       <c r="F2" t="n">
-        <v>36.875</v>
+        <v>37.5</v>
       </c>
       <c r="G2" t="n">
-        <v>10.75</v>
+        <v>11.625</v>
       </c>
       <c r="H2" t="n">
-        <v>3.625</v>
+        <v>3.75</v>
       </c>
       <c r="I2" t="n">
-        <v>52.375</v>
+        <v>52.25</v>
       </c>
       <c r="J2" t="n">
-        <v>37.625</v>
+        <v>37.75</v>
       </c>
       <c r="K2" t="n">
-        <v>112.25</v>
+        <v>111.875</v>
       </c>
       <c r="L2" t="n">
-        <v>26.25</v>
+        <v>25.75</v>
       </c>
       <c r="M2" t="n">
         <v>0</v>
@@ -3577,34 +3577,34 @@
         <v>0</v>
       </c>
       <c r="C3" t="n">
-        <v>112.125</v>
+        <v>113.0625</v>
       </c>
       <c r="D3" t="n">
-        <v>29.0625</v>
+        <v>28.125</v>
       </c>
       <c r="E3" t="n">
         <v>0</v>
       </c>
       <c r="F3" t="n">
-        <v>55.875</v>
+        <v>55.6875</v>
       </c>
       <c r="G3" t="n">
-        <v>16.6875</v>
+        <v>16.875</v>
       </c>
       <c r="H3" t="n">
-        <v>6.375</v>
+        <v>7.5</v>
       </c>
       <c r="I3" t="n">
         <v>78.9375</v>
       </c>
       <c r="J3" t="n">
-        <v>55.6875</v>
+        <v>57.1875</v>
       </c>
       <c r="K3" t="n">
-        <v>167.0625</v>
+        <v>170.25</v>
       </c>
       <c r="L3" t="n">
-        <v>38.0625</v>
+        <v>39.75</v>
       </c>
       <c r="M3" t="n">
         <v>0</v>
@@ -3648,22 +3648,22 @@
         <v>0</v>
       </c>
       <c r="C4" t="n">
-        <v>131.25</v>
+        <v>133.4375</v>
       </c>
       <c r="D4" t="n">
-        <v>33.6875</v>
+        <v>31.71875</v>
       </c>
       <c r="E4" t="n">
         <v>0</v>
       </c>
       <c r="F4" t="n">
-        <v>66.0625</v>
+        <v>66.71875</v>
       </c>
       <c r="G4" t="n">
-        <v>19.6875</v>
+        <v>19.90625</v>
       </c>
       <c r="H4" t="n">
-        <v>5.25</v>
+        <v>5.46875</v>
       </c>
       <c r="I4" t="n">
         <v>91.4375</v>
@@ -3672,10 +3672,10 @@
         <v>65.1875</v>
       </c>
       <c r="K4" t="n">
-        <v>196.65625</v>
+        <v>197.53125</v>
       </c>
       <c r="L4" t="n">
-        <v>47.25</v>
+        <v>46.15625</v>
       </c>
       <c r="M4" t="n">
         <v>0</v>
@@ -3719,34 +3719,34 @@
         <v>0</v>
       </c>
       <c r="C5" t="n">
-        <v>139.921875</v>
+        <v>140.859375</v>
       </c>
       <c r="D5" t="n">
-        <v>35.390625</v>
+        <v>36.328125</v>
       </c>
       <c r="E5" t="n">
         <v>0</v>
       </c>
       <c r="F5" t="n">
-        <v>71.484375</v>
+        <v>71.25</v>
       </c>
       <c r="G5" t="n">
-        <v>20.15625</v>
+        <v>21.09375</v>
       </c>
       <c r="H5" t="n">
-        <v>6.5625</v>
+        <v>8.203125</v>
       </c>
       <c r="I5" t="n">
-        <v>97.96875</v>
+        <v>97.265625</v>
       </c>
       <c r="J5" t="n">
-        <v>71.25</v>
+        <v>70.3125</v>
       </c>
       <c r="K5" t="n">
-        <v>208.59375</v>
+        <v>211.640625</v>
       </c>
       <c r="L5" t="n">
-        <v>49.921875</v>
+        <v>47.34375</v>
       </c>
       <c r="M5" t="n">
         <v>0</v>
@@ -3790,34 +3790,34 @@
         <v>0</v>
       </c>
       <c r="C6" t="n">
-        <v>143.859375</v>
+        <v>146.0390625</v>
       </c>
       <c r="D6" t="n">
-        <v>37.5390625</v>
+        <v>36.5703125</v>
       </c>
       <c r="E6" t="n">
         <v>0</v>
       </c>
       <c r="F6" t="n">
-        <v>74.59375</v>
+        <v>74.109375</v>
       </c>
       <c r="G6" t="n">
-        <v>21.3125</v>
+        <v>21.796875</v>
       </c>
       <c r="H6" t="n">
-        <v>7.5078125</v>
+        <v>6.296875</v>
       </c>
       <c r="I6" t="n">
-        <v>101.234375</v>
+        <v>101.71875</v>
       </c>
       <c r="J6" t="n">
-        <v>71.9296875</v>
+        <v>73.625</v>
       </c>
       <c r="K6" t="n">
-        <v>217.2421875</v>
+        <v>217.7265625</v>
       </c>
       <c r="L6" t="n">
-        <v>49.6484375</v>
+        <v>49.1640625</v>
       </c>
       <c r="M6" t="n">
         <v>0</v>
@@ -3882,7 +3882,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>20109.6</v>
+        <v>20165.6</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -3890,7 +3890,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>209468</v>
+        <v>210196</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -3898,7 +3898,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="n">
-        <v>209468</v>
+        <v>210196</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -3906,7 +3906,7 @@
         <v>3</v>
       </c>
       <c r="B5" t="n">
-        <v>1974984</v>
+        <v>1981848</v>
       </c>
     </row>
   </sheetData>

</xml_diff>